<commit_message>
small changes to American
</commit_message>
<xml_diff>
--- a/AmericanCargo/Test.xlsx
+++ b/AmericanCargo/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\AmericanCargo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\AirCarrierRPA\AmericanCargo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>WONumber</t>
   </si>
@@ -35,67 +35,67 @@
     <t>Waybill Number</t>
   </si>
   <si>
-    <t>001-57980145</t>
-  </si>
-  <si>
-    <t>DJTULA4178739</t>
-  </si>
-  <si>
-    <t>001-58225204</t>
-  </si>
-  <si>
-    <t>DJCLTA4178632</t>
-  </si>
-  <si>
-    <t>001-80731556</t>
-  </si>
-  <si>
-    <t>DJRDUA4178220</t>
-  </si>
-  <si>
-    <t>25M0083740</t>
-  </si>
-  <si>
-    <t>001-59718050</t>
-  </si>
-  <si>
-    <t>DJPHLA4177765</t>
-  </si>
-  <si>
-    <t>001-57931020</t>
-  </si>
-  <si>
-    <t>001-59718735</t>
-  </si>
-  <si>
-    <t>DJINDA4177308</t>
-  </si>
-  <si>
-    <t>21P0159079</t>
-  </si>
-  <si>
-    <t>001-59717770</t>
-  </si>
-  <si>
-    <t>DJAUSA4176649</t>
-  </si>
-  <si>
-    <t>24N0016480</t>
-  </si>
-  <si>
-    <t>001-59342220</t>
-  </si>
-  <si>
-    <t>DJORDA4176509</t>
-  </si>
-  <si>
-    <t>001-58154110</t>
-  </si>
-  <si>
-    <t>DJFLRA4176436</t>
-  </si>
-  <si>
-    <t>001-56733412</t>
+    <t>001-16124695</t>
+  </si>
+  <si>
+    <t>T16600471</t>
+  </si>
+  <si>
+    <t>001-59566426</t>
+  </si>
+  <si>
+    <t>23N0032641</t>
+  </si>
+  <si>
+    <t>001-55655832</t>
+  </si>
+  <si>
+    <t>25M0085133</t>
+  </si>
+  <si>
+    <t>001-59549674</t>
+  </si>
+  <si>
+    <t>001-59718794</t>
+  </si>
+  <si>
+    <t>DJRDUA4279896</t>
+  </si>
+  <si>
+    <t>25M0085202</t>
+  </si>
+  <si>
+    <t>001-20584535</t>
+  </si>
+  <si>
+    <t>DJAUSA4279777</t>
+  </si>
+  <si>
+    <t>24N0016923</t>
+  </si>
+  <si>
+    <t>001-59221260</t>
+  </si>
+  <si>
+    <t>DJLRDA4279757</t>
+  </si>
+  <si>
+    <t>001-20313274</t>
+  </si>
+  <si>
+    <t>DJPHXA4279754</t>
+  </si>
+  <si>
+    <t>001-59521162</t>
+  </si>
+  <si>
+    <t>DJAUSA4279728</t>
+  </si>
+  <si>
+    <t>24N0016913</t>
+  </si>
+  <si>
+    <t>001-59851956</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>223232494</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -456,8 +456,8 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>2250236834</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -468,29 +468,29 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2220563205</v>
       </c>
       <c r="C5">
-        <v>2300257357</v>
+        <v>2220563205</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6">
-        <v>2200249120</v>
-      </c>
-      <c r="C6">
-        <v>2200249120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,30 +511,30 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
+      <c r="C8">
+        <v>211084425</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9">
-        <v>2042801693</v>
+        <v>2110505708</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10">
-        <v>216261908</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,10 +542,10 @@
         <v>23</v>
       </c>
       <c r="B11">
-        <v>2061840883</v>
+        <v>2110505575</v>
       </c>
       <c r="C11">
-        <v>2061840883</v>
+        <v>2110505575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>